<commit_message>
update product admin page
</commit_message>
<xml_diff>
--- a/mysite/hello2.xlsx
+++ b/mysite/hello2.xlsx
@@ -37,610 +37,610 @@
     <t>darrell.skinner5@gmail.com</t>
   </si>
   <si>
+    <t>huibin.hu@brucepower.com</t>
+  </si>
+  <si>
+    <t>helderassuncao@hotmail.com</t>
+  </si>
+  <si>
+    <t>brunobandeiram@hotmail.com</t>
+  </si>
+  <si>
+    <t>amin.maki@gmail.com</t>
+  </si>
+  <si>
+    <t>dreimer.cgy@gmail.com</t>
+  </si>
+  <si>
+    <t>rickertjohn@icloud.com</t>
+  </si>
+  <si>
+    <t>david199130@gmail.com</t>
+  </si>
+  <si>
+    <t>dale.chadney@enbridge.com</t>
+  </si>
+  <si>
+    <t>Ybehnamian@gmail.com</t>
+  </si>
+  <si>
+    <t>amirbehvandi01747@gmail.com</t>
+  </si>
+  <si>
+    <t>elohorakiri@gmail.com</t>
+  </si>
+  <si>
+    <t>lcsouza97@gmail.com</t>
+  </si>
+  <si>
+    <t>mungdx66@gmail.com</t>
+  </si>
+  <si>
+    <t>logan.toth@enbridge.com</t>
+  </si>
+  <si>
+    <t>brook.althouse@arcanite-ndt.com</t>
+  </si>
+  <si>
+    <t>luay.ahmed89@yahoo.com</t>
+  </si>
+  <si>
+    <t>josh_spencer@transcanada.com</t>
+  </si>
+  <si>
+    <t>dstrabel@telus.net</t>
+  </si>
+  <si>
+    <t>derryckm@gmail.com</t>
+  </si>
+  <si>
+    <t>carlb.soares@live.com</t>
+  </si>
+  <si>
+    <t>dheuston@ndtgroup.ca</t>
+  </si>
+  <si>
+    <t>jhetu@ndtgroup.ca</t>
+  </si>
+  <si>
+    <t>maurolcardoso@gmail.com</t>
+  </si>
+  <si>
+    <t>Sohail.anwar@cnrl.com</t>
+  </si>
+  <si>
+    <t>Gengsheng.Weng@cnrl.com</t>
+  </si>
+  <si>
+    <t>twillier@metalogicinspection.com</t>
+  </si>
+  <si>
+    <t>roger.fourny@shaw.ca</t>
+  </si>
+  <si>
+    <t>k.ndt2008@gmail.com</t>
+  </si>
+  <si>
+    <t>mfc_98@hotmail.com</t>
+  </si>
+  <si>
+    <t>mwgumb@bwxt.com</t>
+  </si>
+  <si>
+    <t>justin.knutsen@metalogicinspection.com</t>
+  </si>
+  <si>
+    <t>gford@metalogicinspection.com</t>
+  </si>
+  <si>
+    <t>lebarrozo@gmail.com</t>
+  </si>
+  <si>
+    <t>janalizadeh@gmail.com</t>
+  </si>
+  <si>
+    <t>Nathan.Schuler@cnrl.com</t>
+  </si>
+  <si>
+    <t>elaflamme@nucleom.ca</t>
+  </si>
+  <si>
+    <t>naldenir.amaral@gmail.com</t>
+  </si>
+  <si>
+    <t>dalsaunders@gmail.com</t>
+  </si>
+  <si>
+    <t>natanoel04@hotmail.com</t>
+  </si>
+  <si>
+    <t>marco.venne@gmail.com</t>
+  </si>
+  <si>
+    <t>ideraldo.tiburcio@sbmoffshore.com</t>
+  </si>
+  <si>
+    <t>james.nimijohn@enbridge.com</t>
+  </si>
+  <si>
+    <t>Alex.Arrau@cnrl.com</t>
+  </si>
+  <si>
+    <t>Mandy.Nelson@cnrl.com</t>
+  </si>
+  <si>
+    <t>lucioinspetordm2@gmail.com</t>
+  </si>
+  <si>
+    <t>johnyboyaz@gmail.com</t>
+  </si>
+  <si>
+    <t>marcelo.borchert@sbmoffshore.com</t>
+  </si>
+  <si>
+    <t>robertopintocq@gmail.com</t>
+  </si>
+  <si>
+    <t>Tylor.Arguin@wav.ca</t>
+  </si>
+  <si>
+    <t>Mike.Cook@sbdinc.com</t>
+  </si>
+  <si>
+    <t>Ryan.Faubert@enbridge.com</t>
+  </si>
+  <si>
+    <t>Udaya.Sundar@cnrl.com</t>
+  </si>
+  <si>
+    <t>matthew.prowse@acuren.com</t>
+  </si>
+  <si>
+    <t>homayoun.javadi@tescan.ca</t>
+  </si>
+  <si>
+    <t>David-Tompkins@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mojtaba.ghaderi60@gmail.com</t>
+  </si>
+  <si>
+    <t>noelson.amaral@gmail.com</t>
+  </si>
+  <si>
+    <t>timnelson155@msn.com</t>
+  </si>
+  <si>
+    <t>Michael.Brault@irisndt.com</t>
+  </si>
+  <si>
+    <t>VPopov@nucleom.ca</t>
+  </si>
+  <si>
+    <t>ssinger@acuren.com</t>
+  </si>
+  <si>
+    <t>belchiorvirgilio@gmail.com</t>
+  </si>
+  <si>
+    <t>jodland@tiltinspection.com</t>
+  </si>
+  <si>
+    <t>renatokow@hotmail.com</t>
+  </si>
+  <si>
+    <t>marko.alekszity@gmail.com</t>
+  </si>
+  <si>
+    <t>weston.ellis@opg.com</t>
+  </si>
+  <si>
+    <t>john.reardon@opg.com</t>
+  </si>
+  <si>
+    <t>Brian.Purves@wav.ca</t>
+  </si>
+  <si>
+    <t>kelly.norman@wav.ca</t>
+  </si>
+  <si>
+    <t>mohammad.koochak@gmail.com</t>
+  </si>
+  <si>
+    <t>doubrumm@gmail.com</t>
+  </si>
+  <si>
+    <t>rajasengodan55@gmail.com</t>
+  </si>
+  <si>
+    <t>rgarcia@ndtgroup.ca</t>
+  </si>
+  <si>
+    <t>saramella@gmail.com</t>
+  </si>
+  <si>
+    <t>paul.spencer@applusrtd.com</t>
+  </si>
+  <si>
+    <t>rsb407@gmail.com</t>
+  </si>
+  <si>
+    <t>Philippe.Cyr@acuren.com</t>
+  </si>
+  <si>
+    <t>dana.martin@opg.com</t>
+  </si>
+  <si>
+    <t>Sheryl.vanderfluit@mistrasgroup.com</t>
+  </si>
+  <si>
+    <t>amirghabraee@yahoo.com</t>
+  </si>
+  <si>
+    <t>Jnsmith@bwxt.com</t>
+  </si>
+  <si>
+    <t>wcpamer@bwxt.com</t>
+  </si>
+  <si>
+    <t>practitionerinspection@gmail.com</t>
+  </si>
+  <si>
+    <t>Craig.McMeeken@wav.ca</t>
+  </si>
+  <si>
+    <t>Ben.Ren@cnrl.com</t>
+  </si>
+  <si>
+    <t>Muhammad.Akbar@cnrl.com</t>
+  </si>
+  <si>
+    <t>Hisham.Madi@cnrl.com</t>
+  </si>
+  <si>
+    <t>jtreacy@its-ndt.com</t>
+  </si>
+  <si>
+    <t>dinghaifeng8888@hotmail.com</t>
+  </si>
+  <si>
+    <t>garret.elkins@gmail.com</t>
+  </si>
+  <si>
+    <t>insptonelli@hotmail.com</t>
+  </si>
+  <si>
+    <t>nunomcmarques@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jaeger.Lonsdale@sbdinc.com</t>
+  </si>
+  <si>
+    <t>levikitt@live.ca</t>
+  </si>
+  <si>
+    <t>Bradley.Kuntz@enbridge.com</t>
+  </si>
+  <si>
+    <t>Jay.Brooks@enbridge.com</t>
+  </si>
+  <si>
+    <t>doug.desruisseaux@enbridge.com</t>
+  </si>
+  <si>
+    <t>logan.campbell@enbridge.com</t>
+  </si>
+  <si>
+    <t>darryl.czajkowski@opg.com</t>
+  </si>
+  <si>
+    <t>j.lawson@opg.com</t>
+  </si>
+  <si>
+    <t>derrick.watson@brucepower.com</t>
+  </si>
+  <si>
+    <t>chabouni.djr@gmail.com</t>
+  </si>
+  <si>
+    <t>owen.nicol@enbridge.com</t>
+  </si>
+  <si>
+    <t>dale.berezan@applusrtd.com</t>
+  </si>
+  <si>
+    <t>jian-zhao@hotmail.com</t>
+  </si>
+  <si>
+    <t>scott.robinson@enbridge.com</t>
+  </si>
+  <si>
+    <t>b_ilkuf@hotmail.com</t>
+  </si>
+  <si>
+    <t>douglamarre@sympatico.ca</t>
+  </si>
+  <si>
+    <t>r.hoffmann@rae.com</t>
+  </si>
+  <si>
+    <t>Waleed.Rafiq@cnrl.com</t>
+  </si>
+  <si>
+    <t>Perry.Lawless@cnrl.com</t>
+  </si>
+  <si>
+    <t>Stephen.Orser@cnrl.com</t>
+  </si>
+  <si>
+    <t>Qaiser.Butt@cnrl.com</t>
+  </si>
+  <si>
+    <t>Ayo.Salaudeen@cnrl.com</t>
+  </si>
+  <si>
+    <t>jonathan.Uhlman@cnrl.com</t>
+  </si>
+  <si>
+    <t>Anand.Palani@cnrl.com</t>
+  </si>
+  <si>
+    <t>scott.bangs@brucepower.com</t>
+  </si>
+  <si>
+    <t>tyler.rickard@enbridge.com</t>
+  </si>
+  <si>
+    <t>Zawar.Muhammad@cnrl.com</t>
+  </si>
+  <si>
+    <t>daniel.norman@opg.com</t>
+  </si>
+  <si>
+    <t>hossein.taheri8067@gmail.com</t>
+  </si>
+  <si>
+    <t>matt.fritz@arcanite-ndt.com</t>
+  </si>
+  <si>
+    <t>awallace441@gmail.com</t>
+  </si>
+  <si>
+    <t>joel.djordjevic@arcanite-ndt.com</t>
+  </si>
+  <si>
+    <t>cchartier@ndtgroup.ca</t>
+  </si>
+  <si>
+    <t>humbraganca@hotmail.com</t>
+  </si>
+  <si>
+    <t>flokinn_coq@hotmail.com</t>
+  </si>
+  <si>
+    <t>jmay@ndtgroup.ca</t>
+  </si>
+  <si>
+    <t>marcus.accon@gmail.com</t>
+  </si>
+  <si>
+    <t>ssusac@ndtgroup.ca</t>
+  </si>
+  <si>
+    <t>rackitndt@outlook.com</t>
+  </si>
+  <si>
+    <t>nic.shoebridge@enbridge.com</t>
+  </si>
+  <si>
+    <t>jsaint@metalogicinspection.com</t>
+  </si>
+  <si>
+    <t>blake.macpherson@enbridge.com</t>
+  </si>
+  <si>
+    <t>eng.ndt@yahoo.com</t>
+  </si>
+  <si>
+    <t>h.herrera@rae.com</t>
+  </si>
+  <si>
+    <t>Hassan.Sattar@cnrl.com</t>
+  </si>
+  <si>
+    <t>Marat.Kireev@cnrl.com</t>
+  </si>
+  <si>
+    <t>Alexie.Broddy@cnrl.com</t>
+  </si>
+  <si>
+    <t>nima_vakil@yahoo.com</t>
+  </si>
+  <si>
+    <t>nrweston@anodendt.ca</t>
+  </si>
+  <si>
+    <t>barry.giasson@opg.com</t>
+  </si>
+  <si>
+    <t>michelle.fry@opg.com</t>
+  </si>
+  <si>
+    <t>devon.algera@opg.com</t>
+  </si>
+  <si>
+    <t>briancable40@gmail.com</t>
+  </si>
+  <si>
+    <t>jeehmorais89@gmail.com</t>
+  </si>
+  <si>
+    <t>colbyritzut@gmail.com</t>
+  </si>
+  <si>
+    <t>Dean.Ikert@enbridge.com</t>
+  </si>
+  <si>
+    <t>gabrielvfortes@gmail.com</t>
+  </si>
+  <si>
+    <t>nikhilsatheesan@outlook.com</t>
+  </si>
+  <si>
+    <t>jesse.rempel@enbridge.com</t>
+  </si>
+  <si>
+    <t>karandeepgill760@gmail.com</t>
+  </si>
+  <si>
+    <t>ewhite@ndtgroup.ca</t>
+  </si>
+  <si>
+    <t>collin.coffey@mantech.com</t>
+  </si>
+  <si>
+    <t>Curtis.behnke@enbridge.com</t>
+  </si>
+  <si>
+    <t>marcel@strauhs.com.br</t>
+  </si>
+  <si>
+    <t>ryan.ziefflie@enbridge.com</t>
+  </si>
+  <si>
+    <t>carl.gerbrandt@wav.ca</t>
+  </si>
+  <si>
+    <t>andersonreisssilva@gmail.com</t>
+  </si>
+  <si>
+    <t>gabriell_008@hotmail.com</t>
+  </si>
+  <si>
+    <t>nima.vakilotojjar@gmail.com</t>
+  </si>
+  <si>
+    <t>vinicius.bogos@gmail.com</t>
+  </si>
+  <si>
+    <t>paul.burton@opg.com</t>
+  </si>
+  <si>
+    <t>limogesjon@gmail.com</t>
+  </si>
+  <si>
+    <t>fernando.grigolato@outlook.com</t>
+  </si>
+  <si>
+    <t>nickolas.lau@brucepower.com</t>
+  </si>
+  <si>
+    <t>taylor.gardiner@applusrtd.com</t>
+  </si>
+  <si>
+    <t>srsouzapinto@gmail.com</t>
+  </si>
+  <si>
+    <t>qualidade.daniel@gmail.com</t>
+  </si>
+  <si>
+    <t>ferrerinsp@gmail.com</t>
+  </si>
+  <si>
+    <t>nathaliasg.fr@hotmail.com</t>
+  </si>
+  <si>
+    <t>Jarratt.Bilodeau@StuartOlson.com</t>
+  </si>
+  <si>
+    <t>thiago_claro@hotmail.com</t>
+  </si>
+  <si>
+    <t>julionunescosta@gmail.com</t>
+  </si>
+  <si>
+    <t>chaboki.ali@gmail.com</t>
+  </si>
+  <si>
+    <t>a.beckman94@hotmail.com</t>
+  </si>
+  <si>
+    <t>lacianelli@hotmail.com</t>
+  </si>
+  <si>
+    <t>eng.douglaswilson@yahoo.com.br</t>
+  </si>
+  <si>
+    <t>shawn.hanrahan@opg.com</t>
+  </si>
+  <si>
+    <t>sa-jailson@hotmail.com</t>
+  </si>
+  <si>
+    <t>blessed.agunu@totalenergies.com</t>
+  </si>
+  <si>
+    <t>jrhilson16@gmail.com</t>
+  </si>
+  <si>
+    <t>fqlara@gmail.com</t>
+  </si>
+  <si>
+    <t>mendoncalon@gmail.com</t>
+  </si>
+  <si>
+    <t>oko.oono@gmail.com</t>
+  </si>
+  <si>
+    <t>soheyltahan@gmail.com</t>
+  </si>
+  <si>
+    <t>gmalmeida@isgbrasil.com.br</t>
+  </si>
+  <si>
+    <t>yingsong.wu@applusrtd.com</t>
+  </si>
+  <si>
+    <t>vanderlei_nogueira@hotmail.com</t>
+  </si>
+  <si>
+    <t>felipe@orionsic.com.br</t>
+  </si>
+  <si>
+    <t>eric.scott999@gmail.com</t>
+  </si>
+  <si>
+    <t>brunoinsp@hotmail.com</t>
+  </si>
+  <si>
+    <t>jackbloy@gmail.com</t>
+  </si>
+  <si>
+    <t>rodrigostohler@gmail.com</t>
+  </si>
+  <si>
+    <t>Vptamy@gmail.com</t>
+  </si>
+  <si>
+    <t>diegom.silva@outlook.com</t>
+  </si>
+  <si>
+    <t>felipecadiente@gmail.com</t>
+  </si>
+  <si>
+    <t>marcelo.dimensional@gmail.com</t>
+  </si>
+  <si>
+    <t>wesleyhweber@gmail.com</t>
+  </si>
+  <si>
+    <t>hamed.faghihi@opg.com</t>
+  </si>
+  <si>
+    <t>ben.Leblanc@ultratest.ca</t>
+  </si>
+  <si>
     <t>adam.watkins@enbridge.com</t>
-  </si>
-  <si>
-    <t>huibin.hu@brucepower.com</t>
-  </si>
-  <si>
-    <t>helderassuncao@hotmail.com</t>
-  </si>
-  <si>
-    <t>brunobandeiram@hotmail.com</t>
-  </si>
-  <si>
-    <t>amin.maki@gmail.com</t>
-  </si>
-  <si>
-    <t>dreimer.cgy@gmail.com</t>
-  </si>
-  <si>
-    <t>rickertjohn@icloud.com</t>
-  </si>
-  <si>
-    <t>david199130@gmail.com</t>
-  </si>
-  <si>
-    <t>dale.chadney@enbridge.com</t>
-  </si>
-  <si>
-    <t>Ybehnamian@gmail.com</t>
-  </si>
-  <si>
-    <t>amirbehvandi01747@gmail.com</t>
-  </si>
-  <si>
-    <t>elohorakiri@gmail.com</t>
-  </si>
-  <si>
-    <t>lcsouza97@gmail.com</t>
-  </si>
-  <si>
-    <t>mungdx66@gmail.com</t>
-  </si>
-  <si>
-    <t>logan.toth@enbridge.com</t>
-  </si>
-  <si>
-    <t>brook.althouse@arcanite-ndt.com</t>
-  </si>
-  <si>
-    <t>luay.ahmed89@yahoo.com</t>
-  </si>
-  <si>
-    <t>josh_spencer@transcanada.com</t>
-  </si>
-  <si>
-    <t>dstrabel@telus.net</t>
-  </si>
-  <si>
-    <t>derryckm@gmail.com</t>
-  </si>
-  <si>
-    <t>carlb.soares@live.com</t>
-  </si>
-  <si>
-    <t>dheuston@ndtgroup.ca</t>
-  </si>
-  <si>
-    <t>jhetu@ndtgroup.ca</t>
-  </si>
-  <si>
-    <t>maurolcardoso@gmail.com</t>
-  </si>
-  <si>
-    <t>Sohail.anwar@cnrl.com</t>
-  </si>
-  <si>
-    <t>Gengsheng.Weng@cnrl.com</t>
-  </si>
-  <si>
-    <t>twillier@metalogicinspection.com</t>
-  </si>
-  <si>
-    <t>roger.fourny@shaw.ca</t>
-  </si>
-  <si>
-    <t>k.ndt2008@gmail.com</t>
-  </si>
-  <si>
-    <t>mfc_98@hotmail.com</t>
-  </si>
-  <si>
-    <t>mwgumb@bwxt.com</t>
-  </si>
-  <si>
-    <t>justin.knutsen@metalogicinspection.com</t>
-  </si>
-  <si>
-    <t>gford@metalogicinspection.com</t>
-  </si>
-  <si>
-    <t>lebarrozo@gmail.com</t>
-  </si>
-  <si>
-    <t>janalizadeh@gmail.com</t>
-  </si>
-  <si>
-    <t>Nathan.Schuler@cnrl.com</t>
-  </si>
-  <si>
-    <t>elaflamme@nucleom.ca</t>
-  </si>
-  <si>
-    <t>naldenir.amaral@gmail.com</t>
-  </si>
-  <si>
-    <t>dalsaunders@gmail.com</t>
-  </si>
-  <si>
-    <t>natanoel04@hotmail.com</t>
-  </si>
-  <si>
-    <t>marco.venne@gmail.com</t>
-  </si>
-  <si>
-    <t>ideraldo.tiburcio@sbmoffshore.com</t>
-  </si>
-  <si>
-    <t>james.nimijohn@enbridge.com</t>
-  </si>
-  <si>
-    <t>Alex.Arrau@cnrl.com</t>
-  </si>
-  <si>
-    <t>Mandy.Nelson@cnrl.com</t>
-  </si>
-  <si>
-    <t>lucioinspetordm2@gmail.com</t>
-  </si>
-  <si>
-    <t>johnyboyaz@gmail.com</t>
-  </si>
-  <si>
-    <t>marcelo.borchert@sbmoffshore.com</t>
-  </si>
-  <si>
-    <t>robertopintocq@gmail.com</t>
-  </si>
-  <si>
-    <t>Tylor.Arguin@wav.ca</t>
-  </si>
-  <si>
-    <t>Mike.Cook@sbdinc.com</t>
-  </si>
-  <si>
-    <t>Ryan.Faubert@enbridge.com</t>
-  </si>
-  <si>
-    <t>Udaya.Sundar@cnrl.com</t>
-  </si>
-  <si>
-    <t>matthew.prowse@acuren.com</t>
-  </si>
-  <si>
-    <t>homayoun.javadi@tescan.ca</t>
-  </si>
-  <si>
-    <t>David-Tompkins@hotmail.com</t>
-  </si>
-  <si>
-    <t>Mojtaba.ghaderi60@gmail.com</t>
-  </si>
-  <si>
-    <t>noelson.amaral@gmail.com</t>
-  </si>
-  <si>
-    <t>timnelson155@msn.com</t>
-  </si>
-  <si>
-    <t>Michael.Brault@irisndt.com</t>
-  </si>
-  <si>
-    <t>VPopov@nucleom.ca</t>
-  </si>
-  <si>
-    <t>ssinger@acuren.com</t>
-  </si>
-  <si>
-    <t>belchiorvirgilio@gmail.com</t>
-  </si>
-  <si>
-    <t>jodland@tiltinspection.com</t>
-  </si>
-  <si>
-    <t>renatokow@hotmail.com</t>
-  </si>
-  <si>
-    <t>marko.alekszity@gmail.com</t>
-  </si>
-  <si>
-    <t>weston.ellis@opg.com</t>
-  </si>
-  <si>
-    <t>john.reardon@opg.com</t>
-  </si>
-  <si>
-    <t>Brian.Purves@wav.ca</t>
-  </si>
-  <si>
-    <t>kelly.norman@wav.ca</t>
-  </si>
-  <si>
-    <t>mohammad.koochak@gmail.com</t>
-  </si>
-  <si>
-    <t>doubrumm@gmail.com</t>
-  </si>
-  <si>
-    <t>rajasengodan55@gmail.com</t>
-  </si>
-  <si>
-    <t>rgarcia@ndtgroup.ca</t>
-  </si>
-  <si>
-    <t>saramella@gmail.com</t>
-  </si>
-  <si>
-    <t>paul.spencer@applusrtd.com</t>
-  </si>
-  <si>
-    <t>rsb407@gmail.com</t>
-  </si>
-  <si>
-    <t>Philippe.Cyr@acuren.com</t>
-  </si>
-  <si>
-    <t>dana.martin@opg.com</t>
-  </si>
-  <si>
-    <t>Sheryl.vanderfluit@mistrasgroup.com</t>
-  </si>
-  <si>
-    <t>amirghabraee@yahoo.com</t>
-  </si>
-  <si>
-    <t>Jnsmith@bwxt.com</t>
-  </si>
-  <si>
-    <t>wcpamer@bwxt.com</t>
-  </si>
-  <si>
-    <t>practitionerinspection@gmail.com</t>
-  </si>
-  <si>
-    <t>Craig.McMeeken@wav.ca</t>
-  </si>
-  <si>
-    <t>Ben.Ren@cnrl.com</t>
-  </si>
-  <si>
-    <t>Muhammad.Akbar@cnrl.com</t>
-  </si>
-  <si>
-    <t>Hisham.Madi@cnrl.com</t>
-  </si>
-  <si>
-    <t>jtreacy@its-ndt.com</t>
-  </si>
-  <si>
-    <t>dinghaifeng8888@hotmail.com</t>
-  </si>
-  <si>
-    <t>garret.elkins@gmail.com</t>
-  </si>
-  <si>
-    <t>insptonelli@hotmail.com</t>
-  </si>
-  <si>
-    <t>nunomcmarques@hotmail.com</t>
-  </si>
-  <si>
-    <t>Jaeger.Lonsdale@sbdinc.com</t>
-  </si>
-  <si>
-    <t>levikitt@live.ca</t>
-  </si>
-  <si>
-    <t>Bradley.Kuntz@enbridge.com</t>
-  </si>
-  <si>
-    <t>Jay.Brooks@enbridge.com</t>
-  </si>
-  <si>
-    <t>doug.desruisseaux@enbridge.com</t>
-  </si>
-  <si>
-    <t>logan.campbell@enbridge.com</t>
-  </si>
-  <si>
-    <t>darryl.czajkowski@opg.com</t>
-  </si>
-  <si>
-    <t>j.lawson@opg.com</t>
-  </si>
-  <si>
-    <t>derrick.watson@brucepower.com</t>
-  </si>
-  <si>
-    <t>chabouni.djr@gmail.com</t>
-  </si>
-  <si>
-    <t>owen.nicol@enbridge.com</t>
-  </si>
-  <si>
-    <t>dale.berezan@applusrtd.com</t>
-  </si>
-  <si>
-    <t>jian-zhao@hotmail.com</t>
-  </si>
-  <si>
-    <t>scott.robinson@enbridge.com</t>
-  </si>
-  <si>
-    <t>b_ilkuf@hotmail.com</t>
-  </si>
-  <si>
-    <t>douglamarre@sympatico.ca</t>
-  </si>
-  <si>
-    <t>r.hoffmann@rae.com</t>
-  </si>
-  <si>
-    <t>Waleed.Rafiq@cnrl.com</t>
-  </si>
-  <si>
-    <t>Perry.Lawless@cnrl.com</t>
-  </si>
-  <si>
-    <t>Stephen.Orser@cnrl.com</t>
-  </si>
-  <si>
-    <t>Qaiser.Butt@cnrl.com</t>
-  </si>
-  <si>
-    <t>Ayo.Salaudeen@cnrl.com</t>
-  </si>
-  <si>
-    <t>jonathan.Uhlman@cnrl.com</t>
-  </si>
-  <si>
-    <t>Anand.Palani@cnrl.com</t>
-  </si>
-  <si>
-    <t>scott.bangs@brucepower.com</t>
-  </si>
-  <si>
-    <t>tyler.rickard@enbridge.com</t>
-  </si>
-  <si>
-    <t>Zawar.Muhammad@cnrl.com</t>
-  </si>
-  <si>
-    <t>daniel.norman@opg.com</t>
-  </si>
-  <si>
-    <t>hossein.taheri8067@gmail.com</t>
-  </si>
-  <si>
-    <t>matt.fritz@arcanite-ndt.com</t>
-  </si>
-  <si>
-    <t>awallace441@gmail.com</t>
-  </si>
-  <si>
-    <t>joel.djordjevic@arcanite-ndt.com</t>
-  </si>
-  <si>
-    <t>cchartier@ndtgroup.ca</t>
-  </si>
-  <si>
-    <t>humbraganca@hotmail.com</t>
-  </si>
-  <si>
-    <t>flokinn_coq@hotmail.com</t>
-  </si>
-  <si>
-    <t>jmay@ndtgroup.ca</t>
-  </si>
-  <si>
-    <t>marcus.accon@gmail.com</t>
-  </si>
-  <si>
-    <t>ssusac@ndtgroup.ca</t>
-  </si>
-  <si>
-    <t>rackitndt@outlook.com</t>
-  </si>
-  <si>
-    <t>nic.shoebridge@enbridge.com</t>
-  </si>
-  <si>
-    <t>jsaint@metalogicinspection.com</t>
-  </si>
-  <si>
-    <t>blake.macpherson@enbridge.com</t>
-  </si>
-  <si>
-    <t>eng.ndt@yahoo.com</t>
-  </si>
-  <si>
-    <t>h.herrera@rae.com</t>
-  </si>
-  <si>
-    <t>Hassan.Sattar@cnrl.com</t>
-  </si>
-  <si>
-    <t>Marat.Kireev@cnrl.com</t>
-  </si>
-  <si>
-    <t>Alexie.Broddy@cnrl.com</t>
-  </si>
-  <si>
-    <t>nima_vakil@yahoo.com</t>
-  </si>
-  <si>
-    <t>nrweston@anodendt.ca</t>
-  </si>
-  <si>
-    <t>barry.giasson@opg.com</t>
-  </si>
-  <si>
-    <t>michelle.fry@opg.com</t>
-  </si>
-  <si>
-    <t>devon.algera@opg.com</t>
-  </si>
-  <si>
-    <t>briancable40@gmail.com</t>
-  </si>
-  <si>
-    <t>jeehmorais89@gmail.com</t>
-  </si>
-  <si>
-    <t>colbyritzut@gmail.com</t>
-  </si>
-  <si>
-    <t>Dean.Ikert@enbridge.com</t>
-  </si>
-  <si>
-    <t>gabrielvfortes@gmail.com</t>
-  </si>
-  <si>
-    <t>nikhilsatheesan@outlook.com</t>
-  </si>
-  <si>
-    <t>jesse.rempel@enbridge.com</t>
-  </si>
-  <si>
-    <t>karandeepgill760@gmail.com</t>
-  </si>
-  <si>
-    <t>ewhite@ndtgroup.ca</t>
-  </si>
-  <si>
-    <t>collin.coffey@mantech.com</t>
-  </si>
-  <si>
-    <t>Curtis.behnke@enbridge.com</t>
-  </si>
-  <si>
-    <t>marcel@strauhs.com.br</t>
-  </si>
-  <si>
-    <t>ryan.ziefflie@enbridge.com</t>
-  </si>
-  <si>
-    <t>carl.gerbrandt@wav.ca</t>
-  </si>
-  <si>
-    <t>andersonreisssilva@gmail.com</t>
-  </si>
-  <si>
-    <t>gabriell_008@hotmail.com</t>
-  </si>
-  <si>
-    <t>nima.vakilotojjar@gmail.com</t>
-  </si>
-  <si>
-    <t>vinicius.bogos@gmail.com</t>
-  </si>
-  <si>
-    <t>paul.burton@opg.com</t>
-  </si>
-  <si>
-    <t>limogesjon@gmail.com</t>
-  </si>
-  <si>
-    <t>fernando.grigolato@outlook.com</t>
-  </si>
-  <si>
-    <t>nickolas.lau@brucepower.com</t>
-  </si>
-  <si>
-    <t>taylor.gardiner@applusrtd.com</t>
-  </si>
-  <si>
-    <t>srsouzapinto@gmail.com</t>
-  </si>
-  <si>
-    <t>qualidade.daniel@gmail.com</t>
-  </si>
-  <si>
-    <t>ferrerinsp@gmail.com</t>
-  </si>
-  <si>
-    <t>nathaliasg.fr@hotmail.com</t>
-  </si>
-  <si>
-    <t>Jarratt.Bilodeau@StuartOlson.com</t>
-  </si>
-  <si>
-    <t>thiago_claro@hotmail.com</t>
-  </si>
-  <si>
-    <t>julionunescosta@gmail.com</t>
-  </si>
-  <si>
-    <t>chaboki.ali@gmail.com</t>
-  </si>
-  <si>
-    <t>a.beckman94@hotmail.com</t>
-  </si>
-  <si>
-    <t>lacianelli@hotmail.com</t>
-  </si>
-  <si>
-    <t>eng.douglaswilson@yahoo.com.br</t>
-  </si>
-  <si>
-    <t>shawn.hanrahan@opg.com</t>
-  </si>
-  <si>
-    <t>sa-jailson@hotmail.com</t>
-  </si>
-  <si>
-    <t>jrhilson16@gmail.com</t>
-  </si>
-  <si>
-    <t>fqlara@gmail.com</t>
-  </si>
-  <si>
-    <t>mendoncalon@gmail.com</t>
-  </si>
-  <si>
-    <t>oko.oono@gmail.com</t>
-  </si>
-  <si>
-    <t>soheyltahan@gmail.com</t>
-  </si>
-  <si>
-    <t>gmalmeida@isgbrasil.com.br</t>
-  </si>
-  <si>
-    <t>yingsong.wu@applusrtd.com</t>
-  </si>
-  <si>
-    <t>vanderlei_nogueira@hotmail.com</t>
-  </si>
-  <si>
-    <t>felipe@orionsic.com.br</t>
-  </si>
-  <si>
-    <t>eric.scott999@gmail.com</t>
-  </si>
-  <si>
-    <t>brunoinsp@hotmail.com</t>
-  </si>
-  <si>
-    <t>jackbloy@gmail.com</t>
-  </si>
-  <si>
-    <t>rodrigostohler@gmail.com</t>
-  </si>
-  <si>
-    <t>Vptamy@gmail.com</t>
-  </si>
-  <si>
-    <t>diegom.silva@outlook.com</t>
-  </si>
-  <si>
-    <t>blessed.agunu@totalenergies.com</t>
-  </si>
-  <si>
-    <t>felipecadiente@gmail.com</t>
-  </si>
-  <si>
-    <t>marcelo.dimensional@gmail.com</t>
-  </si>
-  <si>
-    <t>wesleyhweber@gmail.com</t>
-  </si>
-  <si>
-    <t>hamed.faghihi@opg.com</t>
-  </si>
-  <si>
-    <t>ben.Leblanc@ultratest.ca</t>
   </si>
   <si>
     <t>kejqual@telusplanet.net</t>

</xml_diff>